<commit_message>
Actualización de archivos JSON y scripts 22 de octubre
</commit_message>
<xml_diff>
--- a/Proteccion.xlsx
+++ b/Proteccion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="274">
   <si>
     <t>Asignado a</t>
   </si>
@@ -492,9 +492,14 @@
     <t>Ambientación de instancia AWS para migración</t>
   </si>
   <si>
-    <t xml:space="preserve">21/09/2025 Se habilitan todos los accesos para el trabajo en el servidor
+    <t>EN PROCESO</t>
+  </si>
+  <si>
+    <t>21/09/2025 Se habilitan todos los accesos para el trabajo en el servidor
 23/09/2025 Se paro la ejecución debido a tareas con mayor prioridad
-</t>
+07/10/2025 Se empieza de nuevo con la ejecucción de la migración
+10/10/2025 Se encuentra problemas con la comunicación a la base de datos
+15/10/2025 Se genera una nueva instancia de bases de datos que sirva de pruebas para el nuevo ambiente</t>
   </si>
   <si>
     <t>Interno-H14</t>
@@ -503,10 +508,10 @@
     <t>Creación de lógica y vista para la aprobación y rechazos de documentos cargados</t>
   </si>
   <si>
-    <t>EN PROCESO</t>
-  </si>
-  <si>
-    <t>30/09/2025 Este día solo se decdico la mitad del tiempo debido a camnio de prioridades. Se trabajará en el proyecto a medida que se vaya avanzando con las demás tareas</t>
+    <t>30/09/2025 Este día solo se decdico la mitad del tiempo debido a camnio de prioridades. Se trabajará en el proyecto a medida que se vaya avanzando con las demás tareas
+03/10/2025 Debido a la migración, el trabajo se ve reducido a menos de 2 horas diarias para la terminación de este protyecto
+03/10/2025 Se entrega avance y se identifia procesos de mejoras y de añadir operativas para guardar información para cosos de rechazo y de análisis de datos
+14/10/2025 Se entrega avance enfocado en las mejoras de procesos indicadas en la entrega anterior</t>
   </si>
   <si>
     <t>Se necesita la asociación de registros relacionados con pagos de AUF</t>
@@ -527,7 +532,32 @@
     <t xml:space="preserve">Actualización de consumo de mesa unificada para acoplar el flujo nuevo </t>
   </si>
   <si>
-    <t>2/10/2025 Se habilita punto de consumo con las nuevas actualizaciones</t>
+    <t>2/10/2025 Se habilita punto de consumo con las nuevas actualizaciones
+3/10/2025 Se le comunica al cliente para la realización de pruebas</t>
+  </si>
+  <si>
+    <t>REQ-9-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se identifica con ayuda de las pruebas realizadas por el cliente, nuevos procesos para añadir y corregir
+</t>
+  </si>
+  <si>
+    <t>16/10/2025 Se entrega al cliente
+17/10/2025 A la espera de reunión junto con el cliente para finiquitar desarrollo</t>
+  </si>
+  <si>
+    <t>REQ-13-1</t>
+  </si>
+  <si>
+    <t>Se encontraron irregularidaes en validaciones y en el código que deben ser parchadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualización de consumos para la creación de la solicitud de pensión y para el envío de evento de activación de investigación </t>
+  </si>
+  <si>
+    <t>14/10/2025 Se informa desde operación de un caso con bloqueo desde agosto y cuya gestión era prioritaria. Se identifica la problemática y se avanza el caso.
+15/10/2025 Se identifica, por medio de operación, otros problemas que junto con los del día anterior deben ser revisados y parchados</t>
   </si>
   <si>
     <t>Alejandro Cardona Ocampo</t>
@@ -4046,7 +4076,7 @@
       <c r="L20" s="82"/>
       <c r="M20" s="24">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L20, Hoja2!$A$1:$A$18))</f>
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="N20" s="56"/>
       <c r="O20" s="57"/>
@@ -4081,7 +4111,7 @@
       <c r="L21" s="85"/>
       <c r="M21" s="39">
         <f>IF(ISBLANK(L21), NETWORKDAYS(I20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(I20, L21, Hoja2!$A$1:$A$18))</f>
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="N21" s="72"/>
       <c r="O21" s="60"/>
@@ -4365,7 +4395,7 @@
       <c r="L27" s="85"/>
       <c r="M27" s="39">
         <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
-        <v>32793</v>
+        <v>32804</v>
       </c>
       <c r="N27" s="72"/>
       <c r="O27" s="60"/>
@@ -4854,7 +4884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" ht="93.0" customHeight="1">
+    <row r="38" ht="120.75" customHeight="1">
       <c r="A38" s="15" t="s">
         <v>17</v>
       </c>
@@ -4869,13 +4899,13 @@
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="58" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="G38" s="77">
-        <v>30.0</v>
+        <v>85.0</v>
       </c>
       <c r="H38" s="65">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="I38" s="66">
         <v>45910.0</v>
@@ -4889,36 +4919,36 @@
       <c r="L38" s="67"/>
       <c r="M38" s="24">
         <f>IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="N38" s="67"/>
       <c r="O38" s="57"/>
       <c r="P38" s="94" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q38" s="28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="39" ht="76.5" customHeight="1">
+    <row r="39" ht="119.25" customHeight="1">
       <c r="A39" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D39" s="32" t="s">
         <v>130</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="86" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G39" s="34">
-        <v>70.0</v>
+        <v>90.0</v>
       </c>
       <c r="H39" s="48">
         <v>5.0</v>
@@ -4935,7 +4965,7 @@
       <c r="L39" s="71"/>
       <c r="M39" s="39">
         <f>IF(ISBLANK(N39), NETWORKDAYS(J39, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J39, N39, Hoja2!$A$1:$A$18))</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="N39" s="71"/>
       <c r="O39" s="60"/>
@@ -5013,10 +5043,10 @@
       </c>
       <c r="E41" s="32"/>
       <c r="F41" s="86" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G41" s="90">
-        <v>80.0</v>
+        <v>90.0</v>
       </c>
       <c r="H41" s="48">
         <v>3.0</v>
@@ -5030,10 +5060,12 @@
       <c r="K41" s="71">
         <v>45933.0</v>
       </c>
-      <c r="L41" s="71"/>
+      <c r="L41" s="71">
+        <v>45933.0</v>
+      </c>
       <c r="M41" s="39">
         <f>IF(ISBLANK(L41), NETWORKDAYS(J41, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J41, L41, Hoja2!$A$1:$A$18))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N41" s="54">
         <v>45932.0</v>
@@ -5046,87 +5078,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" ht="29.25" customHeight="1">
-      <c r="A42" s="98"/>
-      <c r="B42" s="99"/>
-      <c r="C42" s="100"/>
-      <c r="D42" s="101"/>
-      <c r="E42" s="101"/>
-      <c r="F42" s="102"/>
-      <c r="G42" s="103"/>
-      <c r="H42" s="104"/>
-      <c r="I42" s="105"/>
-      <c r="J42" s="106"/>
-      <c r="K42" s="106"/>
-      <c r="L42" s="106"/>
-      <c r="M42" s="107"/>
-      <c r="N42" s="105"/>
-      <c r="O42" s="108"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="109"/>
-      <c r="R42" s="68"/>
-      <c r="S42" s="68"/>
-      <c r="T42" s="68"/>
-      <c r="U42" s="68"/>
-      <c r="V42" s="68"/>
-      <c r="W42" s="68"/>
-      <c r="X42" s="68"/>
-      <c r="Y42" s="68"/>
-      <c r="Z42" s="68"/>
-      <c r="AA42" s="68"/>
-      <c r="AB42" s="68"/>
-      <c r="AC42" s="68"/>
-      <c r="AD42" s="68"/>
-      <c r="AE42" s="68"/>
-      <c r="AF42" s="68"/>
-      <c r="AG42" s="68"/>
-      <c r="AH42" s="68"/>
-      <c r="AI42" s="68"/>
-      <c r="AJ42" s="68"/>
-      <c r="AK42" s="68"/>
-      <c r="AL42" s="68"/>
-      <c r="AM42" s="69"/>
-    </row>
-    <row r="43" ht="29.25" customHeight="1">
-      <c r="A43" s="110"/>
-      <c r="B43" s="111"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="113"/>
-      <c r="E43" s="113"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="115"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="117"/>
-      <c r="J43" s="118"/>
-      <c r="K43" s="118"/>
-      <c r="L43" s="118"/>
-      <c r="M43" s="119"/>
-      <c r="N43" s="117"/>
-      <c r="O43" s="120"/>
-      <c r="P43" s="61"/>
-      <c r="Q43" s="121"/>
-      <c r="R43" s="61"/>
-      <c r="S43" s="61"/>
-      <c r="T43" s="61"/>
-      <c r="U43" s="61"/>
-      <c r="V43" s="61"/>
-      <c r="W43" s="61"/>
-      <c r="X43" s="61"/>
-      <c r="Y43" s="61"/>
-      <c r="Z43" s="61"/>
-      <c r="AA43" s="61"/>
-      <c r="AB43" s="61"/>
-      <c r="AC43" s="61"/>
-      <c r="AD43" s="61"/>
-      <c r="AE43" s="61"/>
-      <c r="AF43" s="61"/>
-      <c r="AG43" s="61"/>
-      <c r="AH43" s="61"/>
-      <c r="AI43" s="61"/>
-      <c r="AJ43" s="61"/>
-      <c r="AK43" s="61"/>
-      <c r="AL43" s="61"/>
-      <c r="AM43" s="62"/>
+    <row r="42" ht="67.5" customHeight="1">
+      <c r="A42" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="G42" s="77">
+        <v>90.0</v>
+      </c>
+      <c r="H42" s="65">
+        <v>2.0</v>
+      </c>
+      <c r="I42" s="66">
+        <v>45945.0</v>
+      </c>
+      <c r="J42" s="66">
+        <v>45945.0</v>
+      </c>
+      <c r="K42" s="67">
+        <v>45946.0</v>
+      </c>
+      <c r="L42" s="67">
+        <v>45946.0</v>
+      </c>
+      <c r="M42" s="24">
+        <f>IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
+        <v>2</v>
+      </c>
+      <c r="N42" s="67">
+        <v>45946.0</v>
+      </c>
+      <c r="O42" s="57"/>
+      <c r="P42" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q42" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" ht="93.0" customHeight="1">
+      <c r="A43" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="86" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" s="90">
+        <v>60.0</v>
+      </c>
+      <c r="H43" s="48">
+        <v>3.0</v>
+      </c>
+      <c r="I43" s="54">
+        <v>45944.0</v>
+      </c>
+      <c r="J43" s="54">
+        <v>45947.0</v>
+      </c>
+      <c r="K43" s="71">
+        <v>45950.0</v>
+      </c>
+      <c r="L43" s="71"/>
+      <c r="M43" s="39">
+        <f>IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
+      <c r="N43" s="54"/>
+      <c r="O43" s="97"/>
+      <c r="P43" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q43" s="43" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" ht="29.25" customHeight="1">
       <c r="A44" s="98"/>
@@ -42014,19 +42060,19 @@
     </row>
     <row r="2" ht="29.25" customHeight="1">
       <c r="A2" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B2" s="139" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="140" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D2" s="139" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="139" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F2" s="141" t="s">
         <v>21</v>
@@ -42061,19 +42107,19 @@
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B3" s="139" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="140" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D3" s="139" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="139" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="F3" s="141" t="s">
         <v>21</v>
@@ -42108,19 +42154,19 @@
     </row>
     <row r="4" ht="39.0" customHeight="1">
       <c r="A4" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B4" s="139" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="140" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D4" s="139" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="139" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="F4" s="141" t="s">
         <v>21</v>
@@ -42159,19 +42205,19 @@
     </row>
     <row r="5">
       <c r="A5" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B5" s="139" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="140" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D5" s="139" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="155" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="F5" s="141" t="s">
         <v>21</v>
@@ -42210,19 +42256,19 @@
     </row>
     <row r="6" ht="29.25" customHeight="1">
       <c r="A6" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B6" s="139" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="140" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D6" s="139" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F6" s="158" t="s">
         <v>21</v>
@@ -42261,19 +42307,19 @@
     </row>
     <row r="7" ht="29.25" customHeight="1">
       <c r="A7" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B7" s="139" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="140" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D7" s="139" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="139" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F7" s="160" t="s">
         <v>21</v>
@@ -42312,19 +42358,19 @@
     </row>
     <row r="8" ht="29.25" customHeight="1">
       <c r="A8" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B8" s="139" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="140" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D8" s="139" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="162" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F8" s="141" t="s">
         <v>21</v>
@@ -42359,17 +42405,17 @@
     </row>
     <row r="9" ht="29.25" customHeight="1">
       <c r="A9" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B9" s="139" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="166" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="D9" s="167"/>
       <c r="E9" s="139" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="F9" s="160" t="s">
         <v>21</v>
@@ -42406,17 +42452,17 @@
     </row>
     <row r="10" ht="93.0" customHeight="1">
       <c r="A10" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B10" s="139" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="166" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="D10" s="167"/>
       <c r="E10" s="139" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F10" s="160" t="s">
         <v>21</v>
@@ -42451,19 +42497,19 @@
     </row>
     <row r="11">
       <c r="A11" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B11" s="139" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="140" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D11" s="139" t="s">
         <v>41</v>
       </c>
       <c r="E11" s="169" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="F11" s="160" t="s">
         <v>21</v>
@@ -42500,19 +42546,19 @@
     </row>
     <row r="12" ht="29.25" customHeight="1">
       <c r="A12" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B12" s="139" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="170" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D12" s="139" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="139" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F12" s="160" t="s">
         <v>21</v>
@@ -42549,19 +42595,19 @@
     </row>
     <row r="13" ht="29.25" customHeight="1">
       <c r="A13" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B13" s="139" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="166" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D13" s="139" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="139" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F13" s="160" t="s">
         <v>21</v>
@@ -42596,7 +42642,7 @@
     </row>
     <row r="14" ht="29.25" customHeight="1">
       <c r="A14" s="138" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B14" s="139" t="s">
         <v>60</v>
@@ -42606,7 +42652,7 @@
       </c>
       <c r="D14" s="171"/>
       <c r="E14" s="157" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F14" s="165" t="s">
         <v>21</v>
@@ -42684,7 +42730,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="172" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B1" s="172" t="s">
         <v>2</v>
@@ -42711,13 +42757,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="175" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="K1" s="172" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="L1" s="176" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="M1" s="177"/>
       <c r="N1" s="177"/>
@@ -42736,14 +42782,14 @@
     </row>
     <row r="2">
       <c r="A2" s="178" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B2" s="179" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C2" s="180"/>
       <c r="D2" s="181" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E2" s="182">
         <v>45526.0</v>
@@ -42757,7 +42803,7 @@
       <c r="J2" s="180"/>
       <c r="K2" s="180"/>
       <c r="L2" s="180" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="M2" s="183"/>
       <c r="N2" s="183"/>
@@ -42776,13 +42822,13 @@
     </row>
     <row r="3">
       <c r="A3" s="184" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B3" s="185" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C3" s="186" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D3" s="186" t="s">
         <v>21</v>
@@ -42806,7 +42852,7 @@
       </c>
       <c r="K3" s="188"/>
       <c r="L3" s="190" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="M3" s="177"/>
       <c r="N3" s="177"/>
@@ -42825,16 +42871,16 @@
     </row>
     <row r="4">
       <c r="A4" s="191" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B4" s="192" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C4" s="191" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D4" s="193" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E4" s="194">
         <v>45581.0</v>
@@ -42857,7 +42903,7 @@
       </c>
       <c r="K4" s="194"/>
       <c r="L4" s="191" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="M4" s="197"/>
       <c r="N4" s="197"/>
@@ -42876,13 +42922,13 @@
     </row>
     <row r="5">
       <c r="A5" s="176" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B5" s="192" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C5" s="186" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D5" s="198" t="s">
         <v>106</v>
@@ -42906,7 +42952,7 @@
       </c>
       <c r="K5" s="187"/>
       <c r="L5" s="190" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="M5" s="177"/>
       <c r="N5" s="177"/>
@@ -42925,16 +42971,16 @@
     </row>
     <row r="6">
       <c r="A6" s="199" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B6" s="199" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C6" s="193" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D6" s="199" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E6" s="200">
         <v>45602.0</v>
@@ -42955,7 +43001,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="201" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="M6" s="202"/>
       <c r="N6" s="203"/>
@@ -42974,13 +43020,13 @@
     </row>
     <row r="7">
       <c r="A7" s="176" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B7" s="185" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C7" s="204" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D7" s="198" t="s">
         <v>106</v>
@@ -43004,7 +43050,7 @@
       </c>
       <c r="K7" s="198"/>
       <c r="L7" s="206" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="M7" s="207"/>
       <c r="N7" s="207"/>
@@ -43023,14 +43069,14 @@
     </row>
     <row r="8">
       <c r="A8" s="208" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B8" s="209" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C8" s="210"/>
       <c r="D8" s="210" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E8" s="211">
         <v>45603.0</v>
@@ -43051,7 +43097,7 @@
       </c>
       <c r="K8" s="211"/>
       <c r="L8" s="213" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="M8" s="177"/>
       <c r="N8" s="177"/>
@@ -43070,16 +43116,16 @@
     </row>
     <row r="9">
       <c r="A9" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B9" s="215" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C9" s="216" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="D9" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E9" s="218">
         <v>45671.0</v>
@@ -43088,7 +43134,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="216" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="H9" s="218">
         <v>45680.0</v>
@@ -43102,7 +43148,7 @@
       </c>
       <c r="K9" s="216"/>
       <c r="L9" s="220" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M9" s="221"/>
       <c r="N9" s="221"/>
@@ -43121,14 +43167,14 @@
     </row>
     <row r="10">
       <c r="A10" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B10" s="222"/>
       <c r="C10" s="220" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D10" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E10" s="218">
         <v>45671.0</v>
@@ -43147,7 +43193,7 @@
       <c r="J10" s="216"/>
       <c r="K10" s="216"/>
       <c r="L10" s="220" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M10" s="221"/>
       <c r="N10" s="221"/>
@@ -43166,14 +43212,14 @@
     </row>
     <row r="11">
       <c r="A11" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B11" s="222"/>
       <c r="C11" s="220" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D11" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E11" s="218">
         <v>45671.0</v>
@@ -43192,7 +43238,7 @@
       <c r="J11" s="216"/>
       <c r="K11" s="216"/>
       <c r="L11" s="220" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M11" s="221"/>
       <c r="N11" s="221"/>
@@ -43211,14 +43257,14 @@
     </row>
     <row r="12">
       <c r="A12" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B12" s="222"/>
       <c r="C12" s="220" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D12" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E12" s="218">
         <v>45671.0</v>
@@ -43237,7 +43283,7 @@
       <c r="J12" s="216"/>
       <c r="K12" s="216"/>
       <c r="L12" s="220" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M12" s="221"/>
       <c r="N12" s="221"/>
@@ -43256,14 +43302,14 @@
     </row>
     <row r="13">
       <c r="A13" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B13" s="222"/>
       <c r="C13" s="220" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="217" t="s">
         <v>207</v>
-      </c>
-      <c r="D13" s="217" t="s">
-        <v>200</v>
       </c>
       <c r="E13" s="218">
         <v>45671.0</v>
@@ -43282,7 +43328,7 @@
       <c r="J13" s="216"/>
       <c r="K13" s="216"/>
       <c r="L13" s="220" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M13" s="221"/>
       <c r="N13" s="221"/>
@@ -43301,14 +43347,14 @@
     </row>
     <row r="14">
       <c r="A14" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B14" s="222"/>
       <c r="C14" s="220" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D14" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E14" s="218">
         <v>45671.0</v>
@@ -43327,7 +43373,7 @@
       <c r="J14" s="216"/>
       <c r="K14" s="216"/>
       <c r="L14" s="216" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="M14" s="221"/>
       <c r="N14" s="221"/>
@@ -43346,14 +43392,14 @@
     </row>
     <row r="15">
       <c r="A15" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B15" s="222"/>
       <c r="C15" s="220" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D15" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E15" s="218">
         <v>45671.0</v>
@@ -43372,7 +43418,7 @@
       <c r="J15" s="216"/>
       <c r="K15" s="216"/>
       <c r="L15" s="216" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="M15" s="221"/>
       <c r="N15" s="221"/>
@@ -43391,14 +43437,14 @@
     </row>
     <row r="16">
       <c r="A16" s="214" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B16" s="223"/>
       <c r="C16" s="224" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D16" s="217" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E16" s="218">
         <v>45681.0</v>
@@ -43417,7 +43463,7 @@
       <c r="J16" s="216"/>
       <c r="K16" s="216"/>
       <c r="L16" s="220" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="M16" s="221"/>
       <c r="N16" s="221"/>
@@ -49953,7 +49999,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="221" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49961,7 +50007,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="221" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49969,7 +50015,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="221" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49977,7 +50023,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="221" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49985,7 +50031,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="221" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49993,7 +50039,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="221" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -50001,7 +50047,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="221" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -50009,7 +50055,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="221" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -50017,7 +50063,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="221" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -50025,7 +50071,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="221" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -50033,7 +50079,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="221" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -50041,7 +50087,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="221" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -50049,7 +50095,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="221" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -50057,7 +50103,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="221" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -50065,7 +50111,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="221" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -50073,7 +50119,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="221" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -50081,7 +50127,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="221" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -50089,7 +50135,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="221" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -51105,7 +51151,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="226" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B1" s="221"/>
       <c r="C1" s="221"/>
@@ -51163,7 +51209,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="227" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B3" s="228">
         <v>45596.0</v>
@@ -51456,261 +51502,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="231" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B4" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C4" s="233" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="L4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="M4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="N4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="O4" s="234" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="P4" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="R4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="T4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="U4" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="V4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE4" s="236" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="AF4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL4" s="236" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="AM4" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AN4" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AO4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP4" s="236" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="AQ4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS4" s="236" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="AT4" s="237" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AV4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY4" s="236" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="AZ4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BA4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BB4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BH4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI4" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ4" s="236" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="BK4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BL4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BM4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BN4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BO4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BP4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BQ4" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="BR4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BL4" s="235" t="s">
+      <c r="BS4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BM4" s="235" t="s">
+      <c r="BT4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BN4" s="235" t="s">
+      <c r="BU4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BO4" s="235" t="s">
+      <c r="BV4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BP4" s="235" t="s">
+      <c r="BW4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BQ4" s="235" t="s">
+      <c r="BX4" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BR4" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="BS4" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="BT4" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="BU4" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="BV4" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="BW4" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="BX4" s="234" t="s">
-        <v>233</v>
-      </c>
       <c r="BY4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CA4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CB4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CC4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CD4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG4" s="234"/>
       <c r="CH4" s="234"/>
       <c r="CI4" s="236" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="CJ4" s="234"/>
       <c r="CK4" s="234"/>
@@ -51722,249 +51768,249 @@
       <c r="CQ4" s="234"/>
       <c r="CR4" s="234"/>
       <c r="CS4" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="231" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B5" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="L5" s="234" t="s">
+        <v>247</v>
+      </c>
+      <c r="M5" s="234" t="s">
+        <v>247</v>
+      </c>
+      <c r="N5" s="234" t="s">
+        <v>247</v>
+      </c>
+      <c r="O5" s="234" t="s">
+        <v>247</v>
+      </c>
+      <c r="P5" s="235" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q5" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="M5" s="234" t="s">
+      <c r="R5" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="N5" s="234" t="s">
+      <c r="S5" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="O5" s="234" t="s">
+      <c r="T5" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="P5" s="235" t="s">
+      <c r="U5" s="235" t="s">
         <v>240</v>
       </c>
-      <c r="Q5" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="R5" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="S5" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="T5" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="U5" s="235" t="s">
-        <v>233</v>
-      </c>
       <c r="V5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE5" s="238"/>
       <c r="AF5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL5" s="238"/>
       <c r="AM5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AO5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP5" s="238"/>
       <c r="AQ5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AR5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AS5" s="238"/>
       <c r="AT5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AU5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AV5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AW5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AX5" s="234" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="AY5" s="238"/>
       <c r="AZ5" s="234" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA5" s="234" t="s">
         <v>240</v>
       </c>
-      <c r="BA5" s="234" t="s">
-        <v>233</v>
-      </c>
       <c r="BB5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BH5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI5" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ5" s="238"/>
       <c r="BK5" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL5" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN5" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BP5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BQ5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BR5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BS5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BT5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BU5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BX5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BY5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CA5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CB5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CC5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CD5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG5" s="234"/>
       <c r="CH5" s="234"/>
@@ -51979,249 +52025,249 @@
       <c r="CQ5" s="234"/>
       <c r="CR5" s="234"/>
       <c r="CS5" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="231" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B6" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K6" s="239" t="s">
+        <v>249</v>
+      </c>
+      <c r="L6" s="234" t="s">
+        <v>240</v>
+      </c>
+      <c r="M6" s="234" t="s">
+        <v>240</v>
+      </c>
+      <c r="N6" s="234" t="s">
+        <v>240</v>
+      </c>
+      <c r="O6" s="234" t="s">
         <v>242</v>
       </c>
-      <c r="L6" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="M6" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="N6" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="O6" s="234" t="s">
-        <v>235</v>
-      </c>
       <c r="P6" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="R6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="T6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="U6" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="V6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE6" s="238"/>
       <c r="AF6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL6" s="238"/>
       <c r="AM6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AO6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP6" s="238"/>
       <c r="AQ6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS6" s="238"/>
       <c r="AT6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AV6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY6" s="238"/>
       <c r="AZ6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BA6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BB6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BH6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI6" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ6" s="238"/>
       <c r="BK6" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL6" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM6" s="234" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="BN6" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BP6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BQ6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BR6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BS6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BT6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BU6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BX6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BY6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CA6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CB6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CC6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CD6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG6" s="234"/>
       <c r="CH6" s="234"/>
@@ -52236,198 +52282,198 @@
       <c r="CQ6" s="234"/>
       <c r="CR6" s="234"/>
       <c r="CS6" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="231" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B7" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="L7" s="239" t="s">
+        <v>249</v>
+      </c>
+      <c r="M7" s="234" t="s">
+        <v>240</v>
+      </c>
+      <c r="N7" s="234" t="s">
+        <v>240</v>
+      </c>
+      <c r="O7" s="234" t="s">
         <v>242</v>
       </c>
-      <c r="M7" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="N7" s="234" t="s">
-        <v>233</v>
-      </c>
-      <c r="O7" s="234" t="s">
-        <v>235</v>
-      </c>
       <c r="P7" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="R7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="T7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="U7" s="235" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="V7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z7" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AA7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE7" s="238"/>
       <c r="AF7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL7" s="238"/>
       <c r="AM7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AO7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP7" s="238"/>
       <c r="AQ7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS7" s="238"/>
       <c r="AT7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU7" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AV7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY7" s="238"/>
       <c r="AZ7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BA7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BB7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BH7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI7" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ7" s="238"/>
       <c r="BK7" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL7" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN7" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO7" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BP7" s="234"/>
       <c r="BQ7" s="234"/>
@@ -52435,16 +52481,16 @@
       <c r="BS7" s="234"/>
       <c r="BT7" s="234"/>
       <c r="BU7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BX7" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BY7" s="234"/>
       <c r="BZ7" s="234"/>
@@ -52470,220 +52516,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="231" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B8" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="L8" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="M8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="N8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="O8" s="234" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="P8" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="R8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="T8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="U8" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="V8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W8" s="234" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="X8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB8" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AC8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE8" s="238"/>
       <c r="AF8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL8" s="238"/>
       <c r="AM8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN8" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AO8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP8" s="238"/>
       <c r="AQ8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS8" s="238"/>
       <c r="AT8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AV8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY8" s="238"/>
       <c r="AZ8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BA8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BB8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG8" s="234" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="BH8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI8" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ8" s="238"/>
       <c r="BK8" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL8" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN8" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BP8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BQ8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BR8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BS8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BT8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BU8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW8" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BX8" s="234" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="BY8" s="234"/>
       <c r="BZ8" s="234"/>
@@ -52709,244 +52755,244 @@
     </row>
     <row r="9">
       <c r="A9" s="231" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B9" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="L9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="M9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="N9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="O9" s="239" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="P9" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="R9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="T9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="U9" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="V9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE9" s="238"/>
       <c r="AF9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL9" s="238"/>
       <c r="AM9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AO9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP9" s="238"/>
       <c r="AQ9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS9" s="238"/>
       <c r="AT9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AV9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY9" s="238"/>
       <c r="AZ9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BA9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BB9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BH9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI9" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ9" s="238"/>
       <c r="BK9" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL9" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN9" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BP9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BQ9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BR9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BS9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BT9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BU9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BX9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BY9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CA9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CB9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CC9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CD9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG9" s="234"/>
       <c r="CH9" s="234"/>
@@ -52961,249 +53007,249 @@
       <c r="CQ9" s="234"/>
       <c r="CR9" s="234"/>
       <c r="CS9" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="231" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="B10" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="J10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="L10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="M10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="N10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="O10" s="234" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="P10" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="Q10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="R10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="T10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="U10" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="V10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AE10" s="238"/>
       <c r="AF10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AL10" s="238"/>
       <c r="AM10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AN10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AO10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP10" s="238"/>
       <c r="AQ10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS10" s="238"/>
       <c r="AT10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AV10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY10" s="238"/>
       <c r="AZ10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BA10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BB10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BC10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BD10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BE10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BF10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BG10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BH10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI10" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ10" s="238"/>
       <c r="BK10" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL10" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN10" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BP10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BQ10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BR10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BS10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BT10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BU10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW10" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BX10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BY10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CA10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CB10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CC10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CD10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG10" s="234"/>
       <c r="CH10" s="234"/>
@@ -53218,249 +53264,249 @@
       <c r="CQ10" s="234"/>
       <c r="CR10" s="234"/>
       <c r="CS10" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="231" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B11" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="G11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="H11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J11" s="234" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="K11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="L11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="M11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="N11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="O11" s="234" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="P11" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="R11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="S11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="T11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="U11" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="V11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Y11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Z11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AB11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AC11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AE11" s="238"/>
       <c r="AF11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AG11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AH11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AI11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL11" s="238"/>
       <c r="AM11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AN11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AO11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AP11" s="238"/>
       <c r="AQ11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AR11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AS11" s="238"/>
       <c r="AT11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AU11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AV11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AW11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AY11" s="238"/>
       <c r="AZ11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BA11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BB11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BC11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BE11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BF11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BG11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BH11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI11" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BJ11" s="238"/>
       <c r="BK11" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BL11" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BM11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN11" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BO11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BP11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BQ11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BR11" s="234" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="BS11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BT11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BU11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BX11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BY11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CA11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CB11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CC11" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CD11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG11" s="234"/>
       <c r="CH11" s="234"/>
@@ -53475,249 +53521,249 @@
       <c r="CQ11" s="234"/>
       <c r="CR11" s="234"/>
       <c r="CS11" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="231" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="B12" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="G12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="H12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="I12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="J12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="L12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="M12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="N12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="O12" s="234" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="P12" s="235" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="Q12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="R12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="S12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="T12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="U12" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="V12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="W12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="X12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="Y12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="Z12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AA12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AB12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AC12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AE12" s="238"/>
       <c r="AF12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AG12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AH12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AI12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AJ12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AK12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AL12" s="238"/>
       <c r="AM12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AN12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AO12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AP12" s="238"/>
       <c r="AQ12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AR12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AS12" s="238"/>
       <c r="AT12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AU12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AV12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AW12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AX12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AY12" s="238"/>
       <c r="AZ12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BA12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BB12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BC12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BD12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BE12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BF12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BG12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BH12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BI12" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BJ12" s="238"/>
       <c r="BK12" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BL12" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BM12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BN12" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BO12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BP12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BQ12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BR12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BS12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BT12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BU12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BV12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BW12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BX12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BY12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="BZ12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CA12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CB12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CC12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CD12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CE12" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CG12" s="234"/>
       <c r="CH12" s="234"/>
@@ -53732,249 +53778,249 @@
       <c r="CQ12" s="234"/>
       <c r="CR12" s="234"/>
       <c r="CS12" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="231" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B13" s="232" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="F13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="G13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="H13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="I13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="J13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="K13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="L13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="M13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="N13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="O13" s="234" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="P13" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="Q13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="R13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="S13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="T13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="U13" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="V13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="W13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="X13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="Y13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="Z13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AA13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AB13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AC13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AD13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AE13" s="240"/>
       <c r="AF13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AG13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AH13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AI13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="AJ13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AK13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AL13" s="240"/>
       <c r="AM13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AN13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AO13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AP13" s="240"/>
       <c r="AQ13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AR13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AS13" s="240"/>
       <c r="AT13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AU13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AV13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AW13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AX13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="AY13" s="240"/>
       <c r="AZ13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BA13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BB13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BC13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BD13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BE13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BF13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BG13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BH13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BI13" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BJ13" s="240"/>
       <c r="BK13" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BL13" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BM13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BN13" s="235" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BO13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BP13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BQ13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BR13" s="234" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="BS13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BT13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BU13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BV13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BW13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BX13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BY13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="BZ13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CA13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CB13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CC13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="CD13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CE13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CF13" s="234" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="CG13" s="234"/>
       <c r="CH13" s="234"/>
@@ -53989,7 +54035,7 @@
       <c r="CQ13" s="234"/>
       <c r="CR13" s="234"/>
       <c r="CS13" s="234" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -55015,7 +55061,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="241" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B1" s="241" t="s">
         <v>2</v>
@@ -55042,13 +55088,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="245" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="K1" s="246" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="L1" s="244" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="M1" s="247"/>
       <c r="N1" s="247"/>
@@ -55067,10 +55113,10 @@
     </row>
     <row r="2">
       <c r="A2" s="248" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B2" s="249" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C2" s="250"/>
       <c r="D2" s="250" t="s">
@@ -55097,7 +55143,7 @@
       </c>
       <c r="K2" s="253"/>
       <c r="L2" s="254" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="M2" s="247"/>
       <c r="N2" s="247"/>
@@ -55116,16 +55162,16 @@
     </row>
     <row r="3">
       <c r="A3" s="248" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B3" s="255" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C3" s="256" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D3" s="250" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E3" s="251">
         <v>45575.0</v>
@@ -55144,7 +55190,7 @@
       </c>
       <c r="K3" s="251"/>
       <c r="L3" s="254" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="M3" s="257"/>
       <c r="N3" s="247"/>
@@ -55163,14 +55209,14 @@
     </row>
     <row r="4">
       <c r="A4" s="248" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B4" s="238"/>
       <c r="C4" s="258" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D4" s="250" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E4" s="251">
         <v>45575.0</v>
@@ -55189,7 +55235,7 @@
       </c>
       <c r="K4" s="259"/>
       <c r="L4" s="262" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="M4" s="257"/>
       <c r="N4" s="247"/>
@@ -55208,16 +55254,16 @@
     </row>
     <row r="5">
       <c r="A5" s="248" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B5" s="244" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C5" s="250" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="D5" s="250" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E5" s="251">
         <v>45575.0</v>
@@ -55236,7 +55282,7 @@
       </c>
       <c r="K5" s="251"/>
       <c r="L5" s="254" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="M5" s="257"/>
       <c r="N5" s="247"/>

</xml_diff>